<commit_message>
Update data on player pool size to differentiate between swiss and foreign players
</commit_message>
<xml_diff>
--- a/dataAnalysis/tables/playerPoolSize/playerPoolSize.xlsx
+++ b/dataAnalysis/tables/playerPoolSize/playerPoolSize.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5dff752d5d1d42c6/Dokumente/Studium/UniLu/Masterarbeit 2/Masterthesis/dataAnalysis/tables/playerPoolSize/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="11_F25DC773A252ABDACC1048C1511B59885ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E2B263E-4907-46F5-87A1-A5A33CB08299}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="11_F25DC773A252ABDACC1048C1511B59885ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE7D62AC-0639-4F3C-B2EA-742F8B65B1DE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43102" yWindow="-8160" windowWidth="28995" windowHeight="15795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>team</t>
   </si>
   <si>
-    <t>players</t>
-  </si>
-  <si>
     <t>ZSC Lions</t>
   </si>
   <si>
@@ -83,6 +80,15 @@
   </si>
   <si>
     <t>EHC Biel-Bienne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">import </t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>swiss license</t>
   </si>
 </sst>
 </file>
@@ -400,135 +406,238 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" customWidth="1"/>
+    <col min="1" max="3" width="24.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B3">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>22</v>
+      </c>
+      <c r="C11">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>21</v>
+      </c>
+      <c r="C13">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
+      <c r="D13">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>13</v>
-      </c>
-      <c r="B13">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>14</v>
       </c>
       <c r="B14">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>300</v>
+      </c>
+      <c r="C16">
+        <f>SUM(C2:C15)</f>
+        <v>69</v>
+      </c>
+      <c r="D16">
+        <f>SUM(D2:D15)</f>
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>